<commit_message>
actualizacion zonas verdes y arreglo mapa
</commit_message>
<xml_diff>
--- a/zonas_verdes.xlsx
+++ b/zonas_verdes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34644\Documents\Fuentes\Seminario-Fuentes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/59eae136725f9a0b/Documentos/FUENTES DE DATOS/Seminario-Fuentes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587ED3A5-320F-4EFC-AFA7-7C67B5250616}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{587ED3A5-320F-4EFC-AFA7-7C67B5250616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71DBCC0E-B645-445B-BD29-4B193CE61A3C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Población</t>
   </si>
@@ -149,12 +149,51 @@
   <si>
     <t>Balears, Illes</t>
   </si>
+  <si>
+    <t xml:space="preserve">Palma </t>
+  </si>
+  <si>
+    <t>Lugo</t>
+  </si>
+  <si>
+    <t>Huesca</t>
+  </si>
+  <si>
+    <t>Palencia</t>
+  </si>
+  <si>
+    <t>Zamora</t>
+  </si>
+  <si>
+    <t>Cuenca</t>
+  </si>
+  <si>
+    <t>Guadalajara</t>
+  </si>
+  <si>
+    <t>Ciudad Real</t>
+  </si>
+  <si>
+    <t>Cáceres</t>
+  </si>
+  <si>
+    <t>Soria</t>
+  </si>
+  <si>
+    <t>Rioja, La</t>
+  </si>
+  <si>
+    <t>Segovia</t>
+  </si>
+  <si>
+    <t>Ávila</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -205,6 +244,19 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -241,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -263,6 +315,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -278,6 +337,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -481,10 +544,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1692,12 +1755,16 @@
       <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
     </row>
-    <row r="36" spans="1:26" ht="13" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
+    <row r="36" spans="1:26" ht="19" x14ac:dyDescent="0.4">
+      <c r="A36" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="10">
+        <v>406492</v>
+      </c>
+      <c r="C36" s="9">
+        <v>3.42</v>
+      </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -1720,7 +1787,16 @@
       <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
     </row>
-    <row r="37" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" ht="19" x14ac:dyDescent="0.4">
+      <c r="A37" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="10">
+        <v>97211</v>
+      </c>
+      <c r="C37" s="9">
+        <v>6.17</v>
+      </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -1743,7 +1819,18 @@
       <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
     </row>
-    <row r="38" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" ht="19" x14ac:dyDescent="0.4">
+      <c r="A38" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="10">
+        <v>52421</v>
+      </c>
+      <c r="C38" s="9">
+        <v>23.78</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -1766,10 +1853,16 @@
       <c r="Y38" s="3"/>
       <c r="Z38" s="3"/>
     </row>
-    <row r="39" spans="1:26" ht="13" x14ac:dyDescent="0.3">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
+    <row r="39" spans="1:26" ht="19" x14ac:dyDescent="0.4">
+      <c r="A39" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="10">
+        <v>76302</v>
+      </c>
+      <c r="C39" s="9">
+        <v>16.7</v>
+      </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -1794,10 +1887,16 @@
       <c r="Y39" s="3"/>
       <c r="Z39" s="3"/>
     </row>
-    <row r="40" spans="1:26" ht="13" x14ac:dyDescent="0.3">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
+    <row r="40" spans="1:26" ht="19" x14ac:dyDescent="0.4">
+      <c r="A40" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="10">
+        <v>166307</v>
+      </c>
+      <c r="C40" s="9">
+        <v>21</v>
+      </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
@@ -1822,10 +1921,16 @@
       <c r="Y40" s="3"/>
       <c r="Z40" s="3"/>
     </row>
-    <row r="41" spans="1:26" ht="13" x14ac:dyDescent="0.3">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
+    <row r="41" spans="1:26" ht="19" x14ac:dyDescent="0.4">
+      <c r="A41" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="10">
+        <v>198626</v>
+      </c>
+      <c r="C41" s="9">
+        <v>10.46</v>
+      </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -1850,11 +1955,17 @@
       <c r="Y41" s="3"/>
       <c r="Z41" s="3"/>
     </row>
-    <row r="42" spans="1:26" ht="13" x14ac:dyDescent="0.3">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+    <row r="42" spans="1:26" ht="19" x14ac:dyDescent="0.4">
+      <c r="A42" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" s="10">
+        <v>89169</v>
+      </c>
+      <c r="C42" s="9">
+        <v>29</v>
+      </c>
+      <c r="D42" s="11"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
@@ -1878,12 +1989,18 @@
       <c r="Y42" s="3"/>
       <c r="Z42" s="3"/>
     </row>
-    <row r="43" spans="1:26" ht="13" x14ac:dyDescent="0.3">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
+    <row r="43" spans="1:26" ht="19" x14ac:dyDescent="0.4">
+      <c r="A43" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="10">
+        <v>491117</v>
+      </c>
+      <c r="C43" s="9">
+        <v>17.8</v>
+      </c>
       <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
+      <c r="E43" s="11"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -1906,10 +2023,16 @@
       <c r="Y43" s="3"/>
       <c r="Z43" s="3"/>
     </row>
-    <row r="44" spans="1:26" ht="13" x14ac:dyDescent="0.3">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
+    <row r="44" spans="1:26" ht="19" x14ac:dyDescent="0.4">
+      <c r="A44" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="10">
+        <v>95456</v>
+      </c>
+      <c r="C44" s="9">
+        <v>20</v>
+      </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -1934,10 +2057,16 @@
       <c r="Y44" s="3"/>
       <c r="Z44" s="3"/>
     </row>
-    <row r="45" spans="1:26" ht="13" x14ac:dyDescent="0.3">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
+    <row r="45" spans="1:26" ht="19" x14ac:dyDescent="0.4">
+      <c r="A45" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="10">
+        <v>88377</v>
+      </c>
+      <c r="C45" s="9">
+        <v>29.49</v>
+      </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
@@ -1962,10 +2091,16 @@
       <c r="Y45" s="3"/>
       <c r="Z45" s="3"/>
     </row>
-    <row r="46" spans="1:26" ht="13" x14ac:dyDescent="0.3">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
+    <row r="46" spans="1:26" ht="19" x14ac:dyDescent="0.4">
+      <c r="A46" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" s="10">
+        <v>319485</v>
+      </c>
+      <c r="C46" s="9">
+        <v>11.27</v>
+      </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -1990,10 +2125,16 @@
       <c r="Y46" s="3"/>
       <c r="Z46" s="3"/>
     </row>
-    <row r="47" spans="1:26" ht="13" x14ac:dyDescent="0.3">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
+    <row r="47" spans="1:26" ht="19" x14ac:dyDescent="0.4">
+      <c r="A47" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" s="10">
+        <v>153803</v>
+      </c>
+      <c r="C47" s="9">
+        <v>24.05</v>
+      </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -2018,10 +2159,16 @@
       <c r="Y47" s="3"/>
       <c r="Z47" s="3"/>
     </row>
-    <row r="48" spans="1:26" ht="13" x14ac:dyDescent="0.3">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
+    <row r="48" spans="1:26" ht="19" x14ac:dyDescent="0.4">
+      <c r="A48" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" s="10">
+        <v>161771</v>
+      </c>
+      <c r="C48" s="9">
+        <v>25.25</v>
+      </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -2075,11 +2222,6 @@
       <c r="Z49" s="3"/>
     </row>
     <row r="50" spans="1:26" ht="13" x14ac:dyDescent="0.3">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
@@ -2103,6 +2245,11 @@
       <c r="Z50" s="3"/>
     </row>
     <row r="51" spans="1:26" ht="13" x14ac:dyDescent="0.3">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -28669,34 +28816,6 @@
       <c r="Y999" s="3"/>
       <c r="Z999" s="3"/>
     </row>
-    <row r="1000" spans="1:26" ht="13" x14ac:dyDescent="0.3">
-      <c r="A1000" s="3"/>
-      <c r="B1000" s="3"/>
-      <c r="C1000" s="3"/>
-      <c r="D1000" s="3"/>
-      <c r="E1000" s="3"/>
-      <c r="F1000" s="3"/>
-      <c r="G1000" s="3"/>
-      <c r="H1000" s="3"/>
-      <c r="I1000" s="3"/>
-      <c r="J1000" s="3"/>
-      <c r="K1000" s="3"/>
-      <c r="L1000" s="3"/>
-      <c r="M1000" s="3"/>
-      <c r="N1000" s="3"/>
-      <c r="O1000" s="3"/>
-      <c r="P1000" s="3"/>
-      <c r="Q1000" s="3"/>
-      <c r="R1000" s="3"/>
-      <c r="S1000" s="3"/>
-      <c r="T1000" s="3"/>
-      <c r="U1000" s="3"/>
-      <c r="V1000" s="3"/>
-      <c r="W1000" s="3"/>
-      <c r="X1000" s="3"/>
-      <c r="Y1000" s="3"/>
-      <c r="Z1000" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
eliminicación de una celda que he puesto erronea
</commit_message>
<xml_diff>
--- a/zonas_verdes.xlsx
+++ b/zonas_verdes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/59eae136725f9a0b/Documentos/FUENTES DE DATOS/Seminario-Fuentes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34644\Documents\Fuentes\Seminario-Fuentes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{587ED3A5-320F-4EFC-AFA7-7C67B5250616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71DBCC0E-B645-445B-BD29-4B193CE61A3C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2A7965-991A-472C-B547-29373010CEFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Población</t>
   </si>
@@ -84,12 +84,6 @@
     <t>Tarragona</t>
   </si>
   <si>
-    <t>Vigo</t>
-  </si>
-  <si>
-    <t>Palma</t>
-  </si>
-  <si>
     <t>Murcia</t>
   </si>
   <si>
@@ -136,9 +130,6 @@
   </si>
   <si>
     <t>Bizkaia</t>
-  </si>
-  <si>
-    <t>#mirar aproximado</t>
   </si>
   <si>
     <t>Cantabria</t>
@@ -337,10 +328,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -546,15 +533,15 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -588,7 +575,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5">
         <v>246976</v>
@@ -690,7 +677,7 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="5">
         <v>649946</v>
@@ -792,7 +779,7 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B8" s="5">
         <v>581641</v>
@@ -826,7 +813,7 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B9" s="5">
         <v>138144</v>
@@ -894,7 +881,7 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" s="5">
         <v>186370</v>
@@ -928,7 +915,7 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="5">
         <v>272365</v>
@@ -1166,7 +1153,7 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B19" s="5">
         <v>244099</v>
@@ -1268,7 +1255,7 @@
     </row>
     <row r="22" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B22" s="5">
         <v>329988</v>
@@ -1302,7 +1289,7 @@
     </row>
     <row r="23" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B23" s="5">
         <v>214177</v>
@@ -1336,7 +1323,7 @@
     </row>
     <row r="24" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B24" s="5">
         <v>345110</v>
@@ -1345,9 +1332,7 @@
         <v>25.6</v>
       </c>
       <c r="D24" s="6"/>
-      <c r="E24" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -1440,7 +1425,7 @@
     </row>
     <row r="27" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A27" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B27" s="5">
         <v>949471</v>
@@ -1474,7 +1459,7 @@
     </row>
     <row r="28" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B28" s="5">
         <v>377650</v>
@@ -1508,7 +1493,7 @@
     </row>
     <row r="29" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A29" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B29" s="5">
         <v>787808</v>
@@ -1576,7 +1561,7 @@
     </row>
     <row r="31" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B31" s="5">
         <v>569002</v>
@@ -1587,15 +1572,9 @@
       <c r="D31" s="6"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H31" s="5">
-        <v>292986</v>
-      </c>
-      <c r="I31" s="6">
-        <v>3.64</v>
-      </c>
+      <c r="G31" s="4"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="6"/>
       <c r="J31" s="6"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
@@ -1616,7 +1595,7 @@
     </row>
     <row r="32" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A32" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B32" s="5">
         <v>175623</v>
@@ -1627,15 +1606,9 @@
       <c r="D32" s="6"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H32" s="5">
-        <v>406492</v>
-      </c>
-      <c r="I32" s="6">
-        <v>3.42</v>
-      </c>
+      <c r="G32" s="4"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="6"/>
       <c r="J32" s="6"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
@@ -1656,7 +1629,7 @@
     </row>
     <row r="33" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A33" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B33" s="5">
         <v>169498</v>
@@ -1690,7 +1663,7 @@
     </row>
     <row r="34" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A34" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B34" s="5">
         <v>118048</v>
@@ -1724,7 +1697,7 @@
     </row>
     <row r="35" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A35" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B35" s="5">
         <v>1220739</v>
@@ -1757,7 +1730,7 @@
     </row>
     <row r="36" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A36" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B36" s="10">
         <v>406492</v>
@@ -1789,7 +1762,7 @@
     </row>
     <row r="37" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A37" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B37" s="10">
         <v>97211</v>
@@ -1821,7 +1794,7 @@
     </row>
     <row r="38" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A38" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B38" s="10">
         <v>52421</v>
@@ -1855,7 +1828,7 @@
     </row>
     <row r="39" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A39" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B39" s="10">
         <v>76302</v>
@@ -1889,7 +1862,7 @@
     </row>
     <row r="40" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A40" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B40" s="10">
         <v>166307</v>
@@ -1923,7 +1896,7 @@
     </row>
     <row r="41" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A41" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B41" s="10">
         <v>198626</v>
@@ -1957,7 +1930,7 @@
     </row>
     <row r="42" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A42" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B42" s="10">
         <v>89169</v>
@@ -1991,7 +1964,7 @@
     </row>
     <row r="43" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A43" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B43" s="10">
         <v>491117</v>
@@ -2025,7 +1998,7 @@
     </row>
     <row r="44" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A44" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B44" s="10">
         <v>95456</v>
@@ -2059,7 +2032,7 @@
     </row>
     <row r="45" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A45" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B45" s="10">
         <v>88377</v>
@@ -2093,7 +2066,7 @@
     </row>
     <row r="46" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A46" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B46" s="10">
         <v>319485</v>
@@ -2127,7 +2100,7 @@
     </row>
     <row r="47" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A47" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B47" s="10">
         <v>153803</v>
@@ -2161,7 +2134,7 @@
     </row>
     <row r="48" spans="1:26" ht="19" x14ac:dyDescent="0.4">
       <c r="A48" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B48" s="10">
         <v>161771</v>

</xml_diff>